<commit_message>
Updates to Patient and Encounter based on requirements 0.14
</commit_message>
<xml_diff>
--- a/output/nswhealthitocpatient.xlsx
+++ b/output/nswhealthitocpatient.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$196</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$187</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7093" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6767" uniqueCount="602">
   <si>
     <t>Path</t>
   </si>
@@ -1196,18 +1196,6 @@
     <t>The auID identifier value</t>
   </si>
   <si>
-    <t>euID</t>
-  </si>
-  <si>
-    <t>An euID for this patient, as per HIRD: 037 NSW Health Enterprise Unique Person Identifier (EUID)</t>
-  </si>
-  <si>
-    <t>http://ns.health.nsw.gov.au/fhir/ehealth/itoc/id/euid/1.0</t>
-  </si>
-  <si>
-    <t>The euID identifier value</t>
-  </si>
-  <si>
     <t>Patient.active</t>
   </si>
   <si>
@@ -1484,7 +1472,7 @@
 </t>
   </si>
   <si>
-    <t>One or more addresses for the patient.</t>
+    <t>An address for the individual</t>
   </si>
   <si>
     <t>An address for the individual.</t>
@@ -2085,7 +2073,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN196"/>
+  <dimension ref="A1:AN187"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -13582,7 +13570,7 @@
       </c>
       <c r="D101" s="2"/>
       <c r="E101" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F101" t="s" s="2">
         <v>43</v>
@@ -17240,10 +17228,10 @@
       </c>
       <c r="D133" s="2"/>
       <c r="E133" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F133" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G133" t="s" s="2">
         <v>44</v>
@@ -18260,11 +18248,9 @@
     </row>
     <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="B142" t="s" s="2">
         <v>368</v>
       </c>
+      <c r="B142" s="2"/>
       <c r="C142" t="s" s="2">
         <v>44</v>
       </c>
@@ -18279,28 +18265,32 @@
         <v>44</v>
       </c>
       <c r="H142" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I142" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J142" t="s" s="2">
-        <v>133</v>
+        <v>369</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="M142" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="M142" t="s" s="2">
+        <v>372</v>
+      </c>
       <c r="N142" t="s" s="2">
-        <v>136</v>
+        <v>373</v>
       </c>
       <c r="O142" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="P142" s="2"/>
+      <c r="P142" t="s" s="2">
+        <v>374</v>
+      </c>
       <c r="Q142" t="s" s="2">
         <v>44</v>
       </c>
@@ -18344,13 +18334,13 @@
         <v>44</v>
       </c>
       <c r="AE142" t="s" s="2">
-        <v>132</v>
+        <v>368</v>
       </c>
       <c r="AF142" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG142" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH142" t="s" s="2">
         <v>44</v>
@@ -18359,24 +18349,24 @@
         <v>63</v>
       </c>
       <c r="AJ142" t="s" s="2">
-        <v>138</v>
+        <v>375</v>
       </c>
       <c r="AK142" t="s" s="2">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="AL142" t="s" s="2">
-        <v>140</v>
+        <v>376</v>
       </c>
       <c r="AM142" t="s" s="2">
-        <v>141</v>
+        <v>44</v>
       </c>
       <c r="AN142" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="143" hidden="true">
+    <row r="143">
       <c r="A143" t="s" s="2">
-        <v>147</v>
+        <v>377</v>
       </c>
       <c r="B143" s="2"/>
       <c r="C143" t="s" s="2">
@@ -18384,31 +18374,35 @@
       </c>
       <c r="D143" s="2"/>
       <c r="E143" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F143" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G143" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H143" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I143" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J143" t="s" s="2">
-        <v>53</v>
+        <v>378</v>
       </c>
       <c r="K143" t="s" s="2">
-        <v>148</v>
+        <v>379</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="M143" s="2"/>
-      <c r="N143" s="2"/>
+        <v>380</v>
+      </c>
+      <c r="M143" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="N143" t="s" s="2">
+        <v>382</v>
+      </c>
       <c r="O143" t="s" s="2">
         <v>44</v>
       </c>
@@ -18456,31 +18450,31 @@
         <v>44</v>
       </c>
       <c r="AE143" t="s" s="2">
-        <v>150</v>
+        <v>377</v>
       </c>
       <c r="AF143" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG143" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH143" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI143" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ143" t="s" s="2">
-        <v>151</v>
+        <v>383</v>
       </c>
       <c r="AK143" t="s" s="2">
-        <v>44</v>
+        <v>384</v>
       </c>
       <c r="AL143" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM143" t="s" s="2">
-        <v>44</v>
+        <v>385</v>
       </c>
       <c r="AN143" t="s" s="2">
         <v>44</v>
@@ -18488,11 +18482,11 @@
     </row>
     <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
-        <v>152</v>
+        <v>386</v>
       </c>
       <c r="B144" s="2"/>
       <c r="C144" t="s" s="2">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="D144" s="2"/>
       <c r="E144" t="s" s="2">
@@ -18508,21 +18502,23 @@
         <v>44</v>
       </c>
       <c r="I144" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J144" t="s" s="2">
-        <v>96</v>
+        <v>387</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>186</v>
+        <v>388</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>187</v>
+        <v>389</v>
       </c>
       <c r="M144" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N144" s="2"/>
+        <v>390</v>
+      </c>
+      <c r="N144" t="s" s="2">
+        <v>391</v>
+      </c>
       <c r="O144" t="s" s="2">
         <v>44</v>
       </c>
@@ -18558,19 +18554,19 @@
         <v>44</v>
       </c>
       <c r="AA144" t="s" s="2">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="AB144" t="s" s="2">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="AC144" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD144" t="s" s="2">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="AE144" t="s" s="2">
-        <v>154</v>
+        <v>386</v>
       </c>
       <c r="AF144" t="s" s="2">
         <v>42</v>
@@ -18582,19 +18578,19 @@
         <v>44</v>
       </c>
       <c r="AI144" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ144" t="s" s="2">
-        <v>151</v>
+        <v>392</v>
       </c>
       <c r="AK144" t="s" s="2">
-        <v>44</v>
+        <v>393</v>
       </c>
       <c r="AL144" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM144" t="s" s="2">
-        <v>44</v>
+        <v>394</v>
       </c>
       <c r="AN144" t="s" s="2">
         <v>44</v>
@@ -18602,7 +18598,7 @@
     </row>
     <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
-        <v>163</v>
+        <v>395</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" t="s" s="2">
@@ -18619,7 +18615,7 @@
         <v>44</v>
       </c>
       <c r="H145" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I145" t="s" s="2">
         <v>52</v>
@@ -18628,16 +18624,16 @@
         <v>71</v>
       </c>
       <c r="K145" t="s" s="2">
-        <v>164</v>
+        <v>396</v>
       </c>
       <c r="L145" t="s" s="2">
-        <v>165</v>
+        <v>397</v>
       </c>
       <c r="M145" t="s" s="2">
-        <v>166</v>
+        <v>398</v>
       </c>
       <c r="N145" t="s" s="2">
-        <v>167</v>
+        <v>399</v>
       </c>
       <c r="O145" t="s" s="2">
         <v>44</v>
@@ -18665,10 +18661,10 @@
         <v>168</v>
       </c>
       <c r="X145" t="s" s="2">
-        <v>169</v>
+        <v>400</v>
       </c>
       <c r="Y145" t="s" s="2">
-        <v>170</v>
+        <v>401</v>
       </c>
       <c r="Z145" t="s" s="2">
         <v>44</v>
@@ -18686,7 +18682,7 @@
         <v>44</v>
       </c>
       <c r="AE145" t="s" s="2">
-        <v>171</v>
+        <v>395</v>
       </c>
       <c r="AF145" t="s" s="2">
         <v>42</v>
@@ -18701,24 +18697,24 @@
         <v>63</v>
       </c>
       <c r="AJ145" t="s" s="2">
-        <v>172</v>
+        <v>402</v>
       </c>
       <c r="AK145" t="s" s="2">
-        <v>44</v>
+        <v>403</v>
       </c>
       <c r="AL145" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM145" t="s" s="2">
-        <v>94</v>
+        <v>404</v>
       </c>
       <c r="AN145" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="146" hidden="true">
+    <row r="146">
       <c r="A146" t="s" s="2">
-        <v>173</v>
+        <v>405</v>
       </c>
       <c r="B146" s="2"/>
       <c r="C146" t="s" s="2">
@@ -18726,13 +18722,13 @@
       </c>
       <c r="D146" s="2"/>
       <c r="E146" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F146" t="s" s="2">
         <v>51</v>
       </c>
       <c r="G146" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H146" t="s" s="2">
         <v>44</v>
@@ -18741,19 +18737,19 @@
         <v>52</v>
       </c>
       <c r="J146" t="s" s="2">
-        <v>174</v>
+        <v>406</v>
       </c>
       <c r="K146" t="s" s="2">
-        <v>363</v>
+        <v>407</v>
       </c>
       <c r="L146" t="s" s="2">
-        <v>317</v>
+        <v>408</v>
       </c>
       <c r="M146" t="s" s="2">
-        <v>177</v>
+        <v>409</v>
       </c>
       <c r="N146" t="s" s="2">
-        <v>178</v>
+        <v>410</v>
       </c>
       <c r="O146" t="s" s="2">
         <v>44</v>
@@ -18778,13 +18774,13 @@
         <v>44</v>
       </c>
       <c r="W146" t="s" s="2">
-        <v>346</v>
+        <v>44</v>
       </c>
       <c r="X146" t="s" s="2">
-        <v>364</v>
+        <v>44</v>
       </c>
       <c r="Y146" t="s" s="2">
-        <v>365</v>
+        <v>44</v>
       </c>
       <c r="Z146" t="s" s="2">
         <v>44</v>
@@ -18802,7 +18798,7 @@
         <v>44</v>
       </c>
       <c r="AE146" t="s" s="2">
-        <v>182</v>
+        <v>405</v>
       </c>
       <c r="AF146" t="s" s="2">
         <v>42</v>
@@ -18817,24 +18813,24 @@
         <v>63</v>
       </c>
       <c r="AJ146" t="s" s="2">
-        <v>172</v>
+        <v>411</v>
       </c>
       <c r="AK146" t="s" s="2">
-        <v>44</v>
+        <v>412</v>
       </c>
       <c r="AL146" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM146" t="s" s="2">
-        <v>183</v>
+        <v>413</v>
       </c>
       <c r="AN146" t="s" s="2">
-        <v>44</v>
+        <v>414</v>
       </c>
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>206</v>
+        <v>415</v>
       </c>
       <c r="B147" s="2"/>
       <c r="C147" t="s" s="2">
@@ -18842,7 +18838,7 @@
       </c>
       <c r="D147" s="2"/>
       <c r="E147" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F147" t="s" s="2">
         <v>51</v>
@@ -18854,35 +18850,31 @@
         <v>44</v>
       </c>
       <c r="I147" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J147" t="s" s="2">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="K147" t="s" s="2">
-        <v>331</v>
+        <v>416</v>
       </c>
       <c r="L147" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="M147" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="N147" t="s" s="2">
-        <v>210</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="M147" s="2"/>
+      <c r="N147" s="2"/>
       <c r="O147" t="s" s="2">
         <v>44</v>
       </c>
       <c r="P147" s="2"/>
       <c r="Q147" t="s" s="2">
-        <v>370</v>
+        <v>44</v>
       </c>
       <c r="R147" t="s" s="2">
         <v>44</v>
       </c>
       <c r="S147" t="s" s="2">
-        <v>212</v>
+        <v>44</v>
       </c>
       <c r="T147" t="s" s="2">
         <v>44</v>
@@ -18918,7 +18910,7 @@
         <v>44</v>
       </c>
       <c r="AE147" t="s" s="2">
-        <v>213</v>
+        <v>150</v>
       </c>
       <c r="AF147" t="s" s="2">
         <v>42</v>
@@ -18930,10 +18922,10 @@
         <v>44</v>
       </c>
       <c r="AI147" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ147" t="s" s="2">
-        <v>214</v>
+        <v>44</v>
       </c>
       <c r="AK147" t="s" s="2">
         <v>44</v>
@@ -18942,7 +18934,7 @@
         <v>44</v>
       </c>
       <c r="AM147" t="s" s="2">
-        <v>215</v>
+        <v>44</v>
       </c>
       <c r="AN147" t="s" s="2">
         <v>44</v>
@@ -18950,7 +18942,7 @@
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>216</v>
+        <v>418</v>
       </c>
       <c r="B148" s="2"/>
       <c r="C148" t="s" s="2">
@@ -18958,10 +18950,10 @@
       </c>
       <c r="D148" s="2"/>
       <c r="E148" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F148" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G148" t="s" s="2">
         <v>44</v>
@@ -18970,20 +18962,18 @@
         <v>44</v>
       </c>
       <c r="I148" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J148" t="s" s="2">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="K148" t="s" s="2">
-        <v>371</v>
+        <v>97</v>
       </c>
       <c r="L148" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="M148" t="s" s="2">
-        <v>219</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" t="s" s="2">
         <v>44</v>
@@ -18996,7 +18986,7 @@
         <v>44</v>
       </c>
       <c r="S148" t="s" s="2">
-        <v>220</v>
+        <v>44</v>
       </c>
       <c r="T148" t="s" s="2">
         <v>44</v>
@@ -19020,34 +19010,32 @@
         <v>44</v>
       </c>
       <c r="AA148" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB148" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="AB148" s="2"/>
       <c r="AC148" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD148" t="s" s="2">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="AE148" t="s" s="2">
-        <v>222</v>
+        <v>154</v>
       </c>
       <c r="AF148" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG148" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH148" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI148" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ148" t="s" s="2">
-        <v>223</v>
+        <v>44</v>
       </c>
       <c r="AK148" t="s" s="2">
         <v>44</v>
@@ -19056,7 +19044,7 @@
         <v>44</v>
       </c>
       <c r="AM148" t="s" s="2">
-        <v>224</v>
+        <v>44</v>
       </c>
       <c r="AN148" t="s" s="2">
         <v>44</v>
@@ -19064,9 +19052,11 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="B149" s="2"/>
+        <v>418</v>
+      </c>
+      <c r="B149" t="s" s="2">
+        <v>419</v>
+      </c>
       <c r="C149" t="s" s="2">
         <v>44</v>
       </c>
@@ -19084,18 +19074,20 @@
         <v>44</v>
       </c>
       <c r="I149" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J149" t="s" s="2">
-        <v>226</v>
+        <v>420</v>
       </c>
       <c r="K149" t="s" s="2">
-        <v>227</v>
+        <v>421</v>
       </c>
       <c r="L149" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="M149" s="2"/>
+        <v>422</v>
+      </c>
+      <c r="M149" t="s" s="2">
+        <v>423</v>
+      </c>
       <c r="N149" s="2"/>
       <c r="O149" t="s" s="2">
         <v>44</v>
@@ -19144,22 +19136,22 @@
         <v>44</v>
       </c>
       <c r="AE149" t="s" s="2">
-        <v>229</v>
+        <v>154</v>
       </c>
       <c r="AF149" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG149" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH149" t="s" s="2">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="AI149" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ149" t="s" s="2">
-        <v>230</v>
+        <v>44</v>
       </c>
       <c r="AK149" t="s" s="2">
         <v>44</v>
@@ -19168,7 +19160,7 @@
         <v>44</v>
       </c>
       <c r="AM149" t="s" s="2">
-        <v>231</v>
+        <v>44</v>
       </c>
       <c r="AN149" t="s" s="2">
         <v>44</v>
@@ -19176,9 +19168,11 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="B150" s="2"/>
+        <v>418</v>
+      </c>
+      <c r="B150" t="s" s="2">
+        <v>424</v>
+      </c>
       <c r="C150" t="s" s="2">
         <v>44</v>
       </c>
@@ -19196,20 +19190,18 @@
         <v>44</v>
       </c>
       <c r="I150" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J150" t="s" s="2">
-        <v>233</v>
+        <v>425</v>
       </c>
       <c r="K150" t="s" s="2">
-        <v>234</v>
+        <v>426</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M150" t="s" s="2">
-        <v>236</v>
-      </c>
+        <v>427</v>
+      </c>
+      <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" t="s" s="2">
         <v>44</v>
@@ -19258,22 +19250,22 @@
         <v>44</v>
       </c>
       <c r="AE150" t="s" s="2">
-        <v>237</v>
+        <v>154</v>
       </c>
       <c r="AF150" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG150" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH150" t="s" s="2">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="AI150" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ150" t="s" s="2">
-        <v>238</v>
+        <v>44</v>
       </c>
       <c r="AK150" t="s" s="2">
         <v>44</v>
@@ -19282,7 +19274,7 @@
         <v>44</v>
       </c>
       <c r="AM150" t="s" s="2">
-        <v>239</v>
+        <v>44</v>
       </c>
       <c r="AN150" t="s" s="2">
         <v>44</v>
@@ -19290,7 +19282,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>372</v>
+        <v>428</v>
       </c>
       <c r="B151" s="2"/>
       <c r="C151" t="s" s="2">
@@ -19307,32 +19299,26 @@
         <v>44</v>
       </c>
       <c r="H151" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I151" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J151" t="s" s="2">
-        <v>373</v>
+        <v>406</v>
       </c>
       <c r="K151" t="s" s="2">
-        <v>374</v>
+        <v>429</v>
       </c>
       <c r="L151" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="M151" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="N151" t="s" s="2">
-        <v>377</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="M151" s="2"/>
+      <c r="N151" s="2"/>
       <c r="O151" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="P151" t="s" s="2">
-        <v>378</v>
-      </c>
+      <c r="P151" s="2"/>
       <c r="Q151" t="s" s="2">
         <v>44</v>
       </c>
@@ -19376,7 +19362,7 @@
         <v>44</v>
       </c>
       <c r="AE151" t="s" s="2">
-        <v>372</v>
+        <v>431</v>
       </c>
       <c r="AF151" t="s" s="2">
         <v>42</v>
@@ -19388,16 +19374,16 @@
         <v>44</v>
       </c>
       <c r="AI151" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ151" t="s" s="2">
-        <v>379</v>
+        <v>44</v>
       </c>
       <c r="AK151" t="s" s="2">
-        <v>151</v>
+        <v>44</v>
       </c>
       <c r="AL151" t="s" s="2">
-        <v>380</v>
+        <v>44</v>
       </c>
       <c r="AM151" t="s" s="2">
         <v>44</v>
@@ -19406,9 +19392,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>381</v>
+        <v>432</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" t="s" s="2">
@@ -19416,34 +19402,34 @@
       </c>
       <c r="D152" s="2"/>
       <c r="E152" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F152" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G152" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H152" t="s" s="2">
         <v>52</v>
-      </c>
-      <c r="H152" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="I152" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J152" t="s" s="2">
-        <v>382</v>
+        <v>433</v>
       </c>
       <c r="K152" t="s" s="2">
-        <v>383</v>
+        <v>434</v>
       </c>
       <c r="L152" t="s" s="2">
-        <v>384</v>
+        <v>435</v>
       </c>
       <c r="M152" t="s" s="2">
-        <v>385</v>
+        <v>436</v>
       </c>
       <c r="N152" t="s" s="2">
-        <v>386</v>
+        <v>437</v>
       </c>
       <c r="O152" t="s" s="2">
         <v>44</v>
@@ -19480,25 +19466,23 @@
         <v>44</v>
       </c>
       <c r="AA152" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB152" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="AB152" s="2"/>
       <c r="AC152" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD152" t="s" s="2">
-        <v>44</v>
+        <v>439</v>
       </c>
       <c r="AE152" t="s" s="2">
-        <v>381</v>
+        <v>432</v>
       </c>
       <c r="AF152" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG152" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH152" t="s" s="2">
         <v>44</v>
@@ -19507,16 +19491,16 @@
         <v>63</v>
       </c>
       <c r="AJ152" t="s" s="2">
-        <v>387</v>
+        <v>440</v>
       </c>
       <c r="AK152" t="s" s="2">
-        <v>388</v>
+        <v>151</v>
       </c>
       <c r="AL152" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM152" t="s" s="2">
-        <v>389</v>
+        <v>441</v>
       </c>
       <c r="AN152" t="s" s="2">
         <v>44</v>
@@ -19524,9 +19508,11 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="B153" s="2"/>
+        <v>432</v>
+      </c>
+      <c r="B153" t="s" s="2">
+        <v>442</v>
+      </c>
       <c r="C153" t="s" s="2">
         <v>44</v>
       </c>
@@ -19535,31 +19521,31 @@
         <v>42</v>
       </c>
       <c r="F153" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G153" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H153" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I153" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J153" t="s" s="2">
-        <v>391</v>
+        <v>369</v>
       </c>
       <c r="K153" t="s" s="2">
-        <v>392</v>
+        <v>443</v>
       </c>
       <c r="L153" t="s" s="2">
-        <v>393</v>
+        <v>444</v>
       </c>
       <c r="M153" t="s" s="2">
-        <v>394</v>
+        <v>436</v>
       </c>
       <c r="N153" t="s" s="2">
-        <v>395</v>
+        <v>437</v>
       </c>
       <c r="O153" t="s" s="2">
         <v>44</v>
@@ -19608,13 +19594,13 @@
         <v>44</v>
       </c>
       <c r="AE153" t="s" s="2">
-        <v>390</v>
+        <v>432</v>
       </c>
       <c r="AF153" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG153" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH153" t="s" s="2">
         <v>44</v>
@@ -19623,16 +19609,16 @@
         <v>63</v>
       </c>
       <c r="AJ153" t="s" s="2">
-        <v>396</v>
+        <v>440</v>
       </c>
       <c r="AK153" t="s" s="2">
-        <v>397</v>
+        <v>151</v>
       </c>
       <c r="AL153" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM153" t="s" s="2">
-        <v>398</v>
+        <v>441</v>
       </c>
       <c r="AN153" t="s" s="2">
         <v>44</v>
@@ -19640,9 +19626,11 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="B154" s="2"/>
+        <v>432</v>
+      </c>
+      <c r="B154" t="s" s="2">
+        <v>445</v>
+      </c>
       <c r="C154" t="s" s="2">
         <v>44</v>
       </c>
@@ -19657,25 +19645,25 @@
         <v>44</v>
       </c>
       <c r="H154" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I154" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J154" t="s" s="2">
-        <v>71</v>
+        <v>257</v>
       </c>
       <c r="K154" t="s" s="2">
-        <v>400</v>
+        <v>446</v>
       </c>
       <c r="L154" t="s" s="2">
-        <v>401</v>
+        <v>447</v>
       </c>
       <c r="M154" t="s" s="2">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="N154" t="s" s="2">
-        <v>403</v>
+        <v>437</v>
       </c>
       <c r="O154" t="s" s="2">
         <v>44</v>
@@ -19700,13 +19688,13 @@
         <v>44</v>
       </c>
       <c r="W154" t="s" s="2">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="X154" t="s" s="2">
-        <v>404</v>
+        <v>44</v>
       </c>
       <c r="Y154" t="s" s="2">
-        <v>405</v>
+        <v>44</v>
       </c>
       <c r="Z154" t="s" s="2">
         <v>44</v>
@@ -19724,7 +19712,7 @@
         <v>44</v>
       </c>
       <c r="AE154" t="s" s="2">
-        <v>399</v>
+        <v>432</v>
       </c>
       <c r="AF154" t="s" s="2">
         <v>42</v>
@@ -19739,24 +19727,24 @@
         <v>63</v>
       </c>
       <c r="AJ154" t="s" s="2">
-        <v>406</v>
+        <v>440</v>
       </c>
       <c r="AK154" t="s" s="2">
-        <v>407</v>
+        <v>151</v>
       </c>
       <c r="AL154" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM154" t="s" s="2">
-        <v>408</v>
+        <v>441</v>
       </c>
       <c r="AN154" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>409</v>
+        <v>448</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" t="s" s="2">
@@ -19764,35 +19752,31 @@
       </c>
       <c r="D155" s="2"/>
       <c r="E155" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F155" t="s" s="2">
         <v>51</v>
       </c>
       <c r="G155" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H155" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I155" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J155" t="s" s="2">
-        <v>410</v>
+        <v>53</v>
       </c>
       <c r="K155" t="s" s="2">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="L155" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="M155" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="N155" t="s" s="2">
-        <v>414</v>
-      </c>
+        <v>417</v>
+      </c>
+      <c r="M155" s="2"/>
+      <c r="N155" s="2"/>
       <c r="O155" t="s" s="2">
         <v>44</v>
       </c>
@@ -19840,7 +19824,7 @@
         <v>44</v>
       </c>
       <c r="AE155" t="s" s="2">
-        <v>409</v>
+        <v>150</v>
       </c>
       <c r="AF155" t="s" s="2">
         <v>42</v>
@@ -19852,27 +19836,27 @@
         <v>44</v>
       </c>
       <c r="AI155" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ155" t="s" s="2">
-        <v>415</v>
+        <v>44</v>
       </c>
       <c r="AK155" t="s" s="2">
-        <v>416</v>
+        <v>44</v>
       </c>
       <c r="AL155" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM155" t="s" s="2">
-        <v>417</v>
+        <v>44</v>
       </c>
       <c r="AN155" t="s" s="2">
-        <v>418</v>
+        <v>44</v>
       </c>
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>419</v>
+        <v>449</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" t="s" s="2">
@@ -19895,13 +19879,13 @@
         <v>44</v>
       </c>
       <c r="J156" t="s" s="2">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="K156" t="s" s="2">
-        <v>420</v>
+        <v>97</v>
       </c>
       <c r="L156" t="s" s="2">
-        <v>421</v>
+        <v>98</v>
       </c>
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
@@ -19940,31 +19924,29 @@
         <v>44</v>
       </c>
       <c r="AA156" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB156" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="AB156" s="2"/>
       <c r="AC156" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD156" t="s" s="2">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="AE156" t="s" s="2">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="AF156" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG156" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH156" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI156" t="s" s="2">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="AJ156" t="s" s="2">
         <v>44</v>
@@ -19984,9 +19966,11 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="B157" s="2"/>
+        <v>449</v>
+      </c>
+      <c r="B157" t="s" s="2">
+        <v>419</v>
+      </c>
       <c r="C157" t="s" s="2">
         <v>44</v>
       </c>
@@ -19995,7 +19979,7 @@
         <v>42</v>
       </c>
       <c r="F157" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G157" t="s" s="2">
         <v>44</v>
@@ -20007,15 +19991,17 @@
         <v>44</v>
       </c>
       <c r="J157" t="s" s="2">
-        <v>96</v>
+        <v>420</v>
       </c>
       <c r="K157" t="s" s="2">
-        <v>97</v>
+        <v>450</v>
       </c>
       <c r="L157" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="M157" s="2"/>
+        <v>422</v>
+      </c>
+      <c r="M157" t="s" s="2">
+        <v>423</v>
+      </c>
       <c r="N157" s="2"/>
       <c r="O157" t="s" s="2">
         <v>44</v>
@@ -20052,14 +20038,16 @@
         <v>44</v>
       </c>
       <c r="AA157" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AB157" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB157" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC157" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD157" t="s" s="2">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="AE157" t="s" s="2">
         <v>154</v>
@@ -20071,7 +20059,7 @@
         <v>43</v>
       </c>
       <c r="AH157" t="s" s="2">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="AI157" t="s" s="2">
         <v>102</v>
@@ -20094,11 +20082,9 @@
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="B158" t="s" s="2">
-        <v>423</v>
-      </c>
+        <v>451</v>
+      </c>
+      <c r="B158" s="2"/>
       <c r="C158" t="s" s="2">
         <v>44</v>
       </c>
@@ -20119,17 +20105,15 @@
         <v>44</v>
       </c>
       <c r="J158" t="s" s="2">
-        <v>424</v>
+        <v>257</v>
       </c>
       <c r="K158" t="s" s="2">
-        <v>425</v>
+        <v>452</v>
       </c>
       <c r="L158" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="M158" t="s" s="2">
-        <v>427</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" t="s" s="2">
         <v>44</v>
@@ -20178,19 +20162,19 @@
         <v>44</v>
       </c>
       <c r="AE158" t="s" s="2">
-        <v>154</v>
+        <v>453</v>
       </c>
       <c r="AF158" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG158" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH158" t="s" s="2">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="AI158" t="s" s="2">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="AJ158" t="s" s="2">
         <v>44</v>
@@ -20210,11 +20194,9 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="B159" t="s" s="2">
-        <v>428</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="B159" s="2"/>
       <c r="C159" t="s" s="2">
         <v>44</v>
       </c>
@@ -20223,7 +20205,7 @@
         <v>42</v>
       </c>
       <c r="F159" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G159" t="s" s="2">
         <v>44</v>
@@ -20232,19 +20214,23 @@
         <v>44</v>
       </c>
       <c r="I159" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J159" t="s" s="2">
-        <v>429</v>
+        <v>455</v>
       </c>
       <c r="K159" t="s" s="2">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="L159" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="M159" s="2"/>
-      <c r="N159" s="2"/>
+        <v>457</v>
+      </c>
+      <c r="M159" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="N159" t="s" s="2">
+        <v>459</v>
+      </c>
       <c r="O159" t="s" s="2">
         <v>44</v>
       </c>
@@ -20292,7 +20278,7 @@
         <v>44</v>
       </c>
       <c r="AE159" t="s" s="2">
-        <v>154</v>
+        <v>454</v>
       </c>
       <c r="AF159" t="s" s="2">
         <v>42</v>
@@ -20301,22 +20287,22 @@
         <v>43</v>
       </c>
       <c r="AH159" t="s" s="2">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="AI159" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ159" t="s" s="2">
-        <v>44</v>
+        <v>460</v>
       </c>
       <c r="AK159" t="s" s="2">
-        <v>44</v>
+        <v>461</v>
       </c>
       <c r="AL159" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM159" t="s" s="2">
-        <v>44</v>
+        <v>462</v>
       </c>
       <c r="AN159" t="s" s="2">
         <v>44</v>
@@ -20324,7 +20310,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>432</v>
+        <v>463</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" t="s" s="2">
@@ -20347,16 +20333,18 @@
         <v>44</v>
       </c>
       <c r="J160" t="s" s="2">
-        <v>410</v>
+        <v>174</v>
       </c>
       <c r="K160" t="s" s="2">
-        <v>433</v>
+        <v>464</v>
       </c>
       <c r="L160" t="s" s="2">
-        <v>434</v>
+        <v>465</v>
       </c>
       <c r="M160" s="2"/>
-      <c r="N160" s="2"/>
+      <c r="N160" t="s" s="2">
+        <v>466</v>
+      </c>
       <c r="O160" t="s" s="2">
         <v>44</v>
       </c>
@@ -20380,13 +20368,13 @@
         <v>44</v>
       </c>
       <c r="W160" t="s" s="2">
-        <v>44</v>
+        <v>346</v>
       </c>
       <c r="X160" t="s" s="2">
-        <v>44</v>
+        <v>467</v>
       </c>
       <c r="Y160" t="s" s="2">
-        <v>44</v>
+        <v>468</v>
       </c>
       <c r="Z160" t="s" s="2">
         <v>44</v>
@@ -20404,7 +20392,7 @@
         <v>44</v>
       </c>
       <c r="AE160" t="s" s="2">
-        <v>435</v>
+        <v>463</v>
       </c>
       <c r="AF160" t="s" s="2">
         <v>42</v>
@@ -20416,19 +20404,19 @@
         <v>44</v>
       </c>
       <c r="AI160" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ160" t="s" s="2">
-        <v>44</v>
+        <v>469</v>
       </c>
       <c r="AK160" t="s" s="2">
-        <v>44</v>
+        <v>470</v>
       </c>
       <c r="AL160" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM160" t="s" s="2">
-        <v>44</v>
+        <v>471</v>
       </c>
       <c r="AN160" t="s" s="2">
         <v>44</v>
@@ -20436,7 +20424,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>436</v>
+        <v>472</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" t="s" s="2">
@@ -20453,25 +20441,25 @@
         <v>44</v>
       </c>
       <c r="H161" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I161" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J161" t="s" s="2">
-        <v>437</v>
+        <v>473</v>
       </c>
       <c r="K161" t="s" s="2">
-        <v>438</v>
+        <v>474</v>
       </c>
       <c r="L161" t="s" s="2">
-        <v>439</v>
+        <v>475</v>
       </c>
       <c r="M161" t="s" s="2">
-        <v>440</v>
+        <v>476</v>
       </c>
       <c r="N161" t="s" s="2">
-        <v>441</v>
+        <v>477</v>
       </c>
       <c r="O161" t="s" s="2">
         <v>44</v>
@@ -20508,17 +20496,19 @@
         <v>44</v>
       </c>
       <c r="AA161" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="AB161" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB161" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC161" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD161" t="s" s="2">
-        <v>443</v>
+        <v>44</v>
       </c>
       <c r="AE161" t="s" s="2">
-        <v>436</v>
+        <v>472</v>
       </c>
       <c r="AF161" t="s" s="2">
         <v>42</v>
@@ -20533,7 +20523,7 @@
         <v>63</v>
       </c>
       <c r="AJ161" t="s" s="2">
-        <v>444</v>
+        <v>478</v>
       </c>
       <c r="AK161" t="s" s="2">
         <v>151</v>
@@ -20542,7 +20532,7 @@
         <v>44</v>
       </c>
       <c r="AM161" t="s" s="2">
-        <v>445</v>
+        <v>479</v>
       </c>
       <c r="AN161" t="s" s="2">
         <v>44</v>
@@ -20550,11 +20540,9 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="B162" t="s" s="2">
-        <v>446</v>
-      </c>
+        <v>480</v>
+      </c>
+      <c r="B162" s="2"/>
       <c r="C162" t="s" s="2">
         <v>44</v>
       </c>
@@ -20563,31 +20551,31 @@
         <v>42</v>
       </c>
       <c r="F162" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G162" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H162" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I162" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J162" t="s" s="2">
-        <v>373</v>
+        <v>481</v>
       </c>
       <c r="K162" t="s" s="2">
-        <v>447</v>
+        <v>482</v>
       </c>
       <c r="L162" t="s" s="2">
-        <v>448</v>
+        <v>483</v>
       </c>
       <c r="M162" t="s" s="2">
-        <v>440</v>
+        <v>484</v>
       </c>
       <c r="N162" t="s" s="2">
-        <v>441</v>
+        <v>485</v>
       </c>
       <c r="O162" t="s" s="2">
         <v>44</v>
@@ -20636,13 +20624,13 @@
         <v>44</v>
       </c>
       <c r="AE162" t="s" s="2">
-        <v>436</v>
+        <v>480</v>
       </c>
       <c r="AF162" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG162" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH162" t="s" s="2">
         <v>44</v>
@@ -20651,7 +20639,7 @@
         <v>63</v>
       </c>
       <c r="AJ162" t="s" s="2">
-        <v>444</v>
+        <v>486</v>
       </c>
       <c r="AK162" t="s" s="2">
         <v>151</v>
@@ -20660,7 +20648,7 @@
         <v>44</v>
       </c>
       <c r="AM162" t="s" s="2">
-        <v>445</v>
+        <v>487</v>
       </c>
       <c r="AN162" t="s" s="2">
         <v>44</v>
@@ -20668,11 +20656,9 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="B163" t="s" s="2">
-        <v>449</v>
-      </c>
+        <v>488</v>
+      </c>
+      <c r="B163" s="2"/>
       <c r="C163" t="s" s="2">
         <v>44</v>
       </c>
@@ -20681,31 +20667,31 @@
         <v>42</v>
       </c>
       <c r="F163" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G163" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H163" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I163" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J163" t="s" s="2">
-        <v>257</v>
+        <v>489</v>
       </c>
       <c r="K163" t="s" s="2">
-        <v>450</v>
+        <v>490</v>
       </c>
       <c r="L163" t="s" s="2">
-        <v>451</v>
+        <v>491</v>
       </c>
       <c r="M163" t="s" s="2">
-        <v>440</v>
+        <v>492</v>
       </c>
       <c r="N163" t="s" s="2">
-        <v>441</v>
+        <v>493</v>
       </c>
       <c r="O163" t="s" s="2">
         <v>44</v>
@@ -20754,22 +20740,22 @@
         <v>44</v>
       </c>
       <c r="AE163" t="s" s="2">
-        <v>436</v>
+        <v>488</v>
       </c>
       <c r="AF163" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG163" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH163" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI163" t="s" s="2">
-        <v>63</v>
+        <v>494</v>
       </c>
       <c r="AJ163" t="s" s="2">
-        <v>444</v>
+        <v>495</v>
       </c>
       <c r="AK163" t="s" s="2">
         <v>151</v>
@@ -20778,7 +20764,7 @@
         <v>44</v>
       </c>
       <c r="AM163" t="s" s="2">
-        <v>445</v>
+        <v>44</v>
       </c>
       <c r="AN163" t="s" s="2">
         <v>44</v>
@@ -20786,7 +20772,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>452</v>
+        <v>496</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" t="s" s="2">
@@ -20812,10 +20798,10 @@
         <v>53</v>
       </c>
       <c r="K164" t="s" s="2">
-        <v>420</v>
+        <v>148</v>
       </c>
       <c r="L164" t="s" s="2">
-        <v>421</v>
+        <v>149</v>
       </c>
       <c r="M164" s="2"/>
       <c r="N164" s="2"/>
@@ -20881,7 +20867,7 @@
         <v>44</v>
       </c>
       <c r="AJ164" t="s" s="2">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="AK164" t="s" s="2">
         <v>44</v>
@@ -20898,18 +20884,18 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>453</v>
+        <v>497</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" t="s" s="2">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="D165" s="2"/>
       <c r="E165" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F165" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G165" t="s" s="2">
         <v>44</v>
@@ -20924,12 +20910,14 @@
         <v>96</v>
       </c>
       <c r="K165" t="s" s="2">
-        <v>97</v>
+        <v>186</v>
       </c>
       <c r="L165" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="M165" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="M165" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N165" s="2"/>
       <c r="O165" t="s" s="2">
         <v>44</v>
@@ -20966,14 +20954,16 @@
         <v>44</v>
       </c>
       <c r="AA165" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AB165" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="AB165" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="AC165" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD165" t="s" s="2">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="AE165" t="s" s="2">
         <v>154</v>
@@ -20991,7 +20981,7 @@
         <v>102</v>
       </c>
       <c r="AJ165" t="s" s="2">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="AK165" t="s" s="2">
         <v>44</v>
@@ -21008,43 +20998,43 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>453</v>
-      </c>
-      <c r="B166" t="s" s="2">
-        <v>423</v>
-      </c>
+        <v>498</v>
+      </c>
+      <c r="B166" s="2"/>
       <c r="C166" t="s" s="2">
-        <v>44</v>
+        <v>499</v>
       </c>
       <c r="D166" s="2"/>
       <c r="E166" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F166" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G166" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H166" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I166" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J166" t="s" s="2">
-        <v>424</v>
+        <v>96</v>
       </c>
       <c r="K166" t="s" s="2">
-        <v>454</v>
+        <v>500</v>
       </c>
       <c r="L166" t="s" s="2">
-        <v>426</v>
+        <v>501</v>
       </c>
       <c r="M166" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="N166" s="2"/>
+        <v>129</v>
+      </c>
+      <c r="N166" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O166" t="s" s="2">
         <v>44</v>
       </c>
@@ -21092,7 +21082,7 @@
         <v>44</v>
       </c>
       <c r="AE166" t="s" s="2">
-        <v>154</v>
+        <v>502</v>
       </c>
       <c r="AF166" t="s" s="2">
         <v>42</v>
@@ -21101,13 +21091,13 @@
         <v>43</v>
       </c>
       <c r="AH166" t="s" s="2">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="AI166" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ166" t="s" s="2">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="AK166" t="s" s="2">
         <v>44</v>
@@ -21124,7 +21114,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>455</v>
+        <v>503</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" t="s" s="2">
@@ -21135,7 +21125,7 @@
         <v>42</v>
       </c>
       <c r="F167" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G167" t="s" s="2">
         <v>44</v>
@@ -21147,16 +21137,18 @@
         <v>44</v>
       </c>
       <c r="J167" t="s" s="2">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="K167" t="s" s="2">
-        <v>456</v>
+        <v>504</v>
       </c>
       <c r="L167" t="s" s="2">
-        <v>434</v>
+        <v>505</v>
       </c>
       <c r="M167" s="2"/>
-      <c r="N167" s="2"/>
+      <c r="N167" t="s" s="2">
+        <v>506</v>
+      </c>
       <c r="O167" t="s" s="2">
         <v>44</v>
       </c>
@@ -21180,13 +21172,13 @@
         <v>44</v>
       </c>
       <c r="W167" t="s" s="2">
-        <v>44</v>
+        <v>346</v>
       </c>
       <c r="X167" t="s" s="2">
-        <v>44</v>
+        <v>507</v>
       </c>
       <c r="Y167" t="s" s="2">
-        <v>44</v>
+        <v>508</v>
       </c>
       <c r="Z167" t="s" s="2">
         <v>44</v>
@@ -21204,39 +21196,39 @@
         <v>44</v>
       </c>
       <c r="AE167" t="s" s="2">
-        <v>457</v>
+        <v>503</v>
       </c>
       <c r="AF167" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG167" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH167" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI167" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ167" t="s" s="2">
-        <v>44</v>
+        <v>509</v>
       </c>
       <c r="AK167" t="s" s="2">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="AL167" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM167" t="s" s="2">
-        <v>44</v>
+        <v>510</v>
       </c>
       <c r="AN167" t="s" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>458</v>
+        <v>511</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" t="s" s="2">
@@ -21244,34 +21236,32 @@
       </c>
       <c r="D168" s="2"/>
       <c r="E168" t="s" s="2">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F168" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G168" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H168" t="s" s="2">
         <v>44</v>
       </c>
       <c r="I168" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J168" t="s" s="2">
-        <v>459</v>
+        <v>378</v>
       </c>
       <c r="K168" t="s" s="2">
-        <v>460</v>
+        <v>512</v>
       </c>
       <c r="L168" t="s" s="2">
-        <v>461</v>
-      </c>
-      <c r="M168" t="s" s="2">
-        <v>462</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="M168" s="2"/>
       <c r="N168" t="s" s="2">
-        <v>463</v>
+        <v>514</v>
       </c>
       <c r="O168" t="s" s="2">
         <v>44</v>
@@ -21320,13 +21310,13 @@
         <v>44</v>
       </c>
       <c r="AE168" t="s" s="2">
-        <v>458</v>
+        <v>511</v>
       </c>
       <c r="AF168" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG168" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH168" t="s" s="2">
         <v>44</v>
@@ -21335,16 +21325,16 @@
         <v>63</v>
       </c>
       <c r="AJ168" t="s" s="2">
-        <v>464</v>
+        <v>383</v>
       </c>
       <c r="AK168" t="s" s="2">
-        <v>465</v>
+        <v>151</v>
       </c>
       <c r="AL168" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM168" t="s" s="2">
-        <v>466</v>
+        <v>515</v>
       </c>
       <c r="AN168" t="s" s="2">
         <v>44</v>
@@ -21352,7 +21342,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>467</v>
+        <v>516</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" t="s" s="2">
@@ -21363,7 +21353,7 @@
         <v>42</v>
       </c>
       <c r="F169" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G169" t="s" s="2">
         <v>44</v>
@@ -21375,17 +21365,19 @@
         <v>44</v>
       </c>
       <c r="J169" t="s" s="2">
-        <v>174</v>
+        <v>387</v>
       </c>
       <c r="K169" t="s" s="2">
-        <v>468</v>
+        <v>517</v>
       </c>
       <c r="L169" t="s" s="2">
-        <v>469</v>
-      </c>
-      <c r="M169" s="2"/>
+        <v>518</v>
+      </c>
+      <c r="M169" t="s" s="2">
+        <v>519</v>
+      </c>
       <c r="N169" t="s" s="2">
-        <v>470</v>
+        <v>391</v>
       </c>
       <c r="O169" t="s" s="2">
         <v>44</v>
@@ -21410,13 +21402,13 @@
         <v>44</v>
       </c>
       <c r="W169" t="s" s="2">
-        <v>346</v>
+        <v>44</v>
       </c>
       <c r="X169" t="s" s="2">
-        <v>471</v>
+        <v>44</v>
       </c>
       <c r="Y169" t="s" s="2">
-        <v>472</v>
+        <v>44</v>
       </c>
       <c r="Z169" t="s" s="2">
         <v>44</v>
@@ -21434,13 +21426,13 @@
         <v>44</v>
       </c>
       <c r="AE169" t="s" s="2">
-        <v>467</v>
+        <v>516</v>
       </c>
       <c r="AF169" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG169" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH169" t="s" s="2">
         <v>44</v>
@@ -21449,16 +21441,16 @@
         <v>63</v>
       </c>
       <c r="AJ169" t="s" s="2">
-        <v>473</v>
+        <v>392</v>
       </c>
       <c r="AK169" t="s" s="2">
-        <v>474</v>
+        <v>151</v>
       </c>
       <c r="AL169" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM169" t="s" s="2">
-        <v>475</v>
+        <v>520</v>
       </c>
       <c r="AN169" t="s" s="2">
         <v>44</v>
@@ -21466,7 +21458,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>476</v>
+        <v>521</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" t="s" s="2">
@@ -21489,19 +21481,17 @@
         <v>44</v>
       </c>
       <c r="J170" t="s" s="2">
-        <v>477</v>
+        <v>455</v>
       </c>
       <c r="K170" t="s" s="2">
-        <v>478</v>
+        <v>522</v>
       </c>
       <c r="L170" t="s" s="2">
-        <v>479</v>
-      </c>
-      <c r="M170" t="s" s="2">
-        <v>480</v>
-      </c>
+        <v>523</v>
+      </c>
+      <c r="M170" s="2"/>
       <c r="N170" t="s" s="2">
-        <v>481</v>
+        <v>524</v>
       </c>
       <c r="O170" t="s" s="2">
         <v>44</v>
@@ -21550,7 +21540,7 @@
         <v>44</v>
       </c>
       <c r="AE170" t="s" s="2">
-        <v>476</v>
+        <v>521</v>
       </c>
       <c r="AF170" t="s" s="2">
         <v>42</v>
@@ -21565,7 +21555,7 @@
         <v>63</v>
       </c>
       <c r="AJ170" t="s" s="2">
-        <v>482</v>
+        <v>460</v>
       </c>
       <c r="AK170" t="s" s="2">
         <v>151</v>
@@ -21574,7 +21564,7 @@
         <v>44</v>
       </c>
       <c r="AM170" t="s" s="2">
-        <v>483</v>
+        <v>525</v>
       </c>
       <c r="AN170" t="s" s="2">
         <v>44</v>
@@ -21582,7 +21572,7 @@
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="B171" s="2"/>
       <c r="C171" t="s" s="2">
@@ -21593,7 +21583,7 @@
         <v>42</v>
       </c>
       <c r="F171" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G171" t="s" s="2">
         <v>44</v>
@@ -21605,19 +21595,17 @@
         <v>44</v>
       </c>
       <c r="J171" t="s" s="2">
-        <v>485</v>
+        <v>71</v>
       </c>
       <c r="K171" t="s" s="2">
-        <v>486</v>
+        <v>396</v>
       </c>
       <c r="L171" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="M171" t="s" s="2">
-        <v>488</v>
-      </c>
+        <v>527</v>
+      </c>
+      <c r="M171" s="2"/>
       <c r="N171" t="s" s="2">
-        <v>489</v>
+        <v>528</v>
       </c>
       <c r="O171" t="s" s="2">
         <v>44</v>
@@ -21642,13 +21630,13 @@
         <v>44</v>
       </c>
       <c r="W171" t="s" s="2">
-        <v>44</v>
+        <v>168</v>
       </c>
       <c r="X171" t="s" s="2">
-        <v>44</v>
+        <v>400</v>
       </c>
       <c r="Y171" t="s" s="2">
-        <v>44</v>
+        <v>401</v>
       </c>
       <c r="Z171" t="s" s="2">
         <v>44</v>
@@ -21666,13 +21654,13 @@
         <v>44</v>
       </c>
       <c r="AE171" t="s" s="2">
-        <v>484</v>
+        <v>526</v>
       </c>
       <c r="AF171" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG171" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH171" t="s" s="2">
         <v>44</v>
@@ -21681,7 +21669,7 @@
         <v>63</v>
       </c>
       <c r="AJ171" t="s" s="2">
-        <v>490</v>
+        <v>402</v>
       </c>
       <c r="AK171" t="s" s="2">
         <v>151</v>
@@ -21690,7 +21678,7 @@
         <v>44</v>
       </c>
       <c r="AM171" t="s" s="2">
-        <v>491</v>
+        <v>529</v>
       </c>
       <c r="AN171" t="s" s="2">
         <v>44</v>
@@ -21698,7 +21686,7 @@
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>492</v>
+        <v>530</v>
       </c>
       <c r="B172" s="2"/>
       <c r="C172" t="s" s="2">
@@ -21709,7 +21697,7 @@
         <v>42</v>
       </c>
       <c r="F172" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G172" t="s" s="2">
         <v>44</v>
@@ -21721,19 +21709,17 @@
         <v>44</v>
       </c>
       <c r="J172" t="s" s="2">
-        <v>493</v>
+        <v>233</v>
       </c>
       <c r="K172" t="s" s="2">
-        <v>494</v>
+        <v>531</v>
       </c>
       <c r="L172" t="s" s="2">
-        <v>495</v>
-      </c>
-      <c r="M172" t="s" s="2">
-        <v>496</v>
-      </c>
+        <v>532</v>
+      </c>
+      <c r="M172" s="2"/>
       <c r="N172" t="s" s="2">
-        <v>497</v>
+        <v>533</v>
       </c>
       <c r="O172" t="s" s="2">
         <v>44</v>
@@ -21782,22 +21768,22 @@
         <v>44</v>
       </c>
       <c r="AE172" t="s" s="2">
-        <v>492</v>
+        <v>530</v>
       </c>
       <c r="AF172" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG172" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH172" t="s" s="2">
-        <v>44</v>
+        <v>534</v>
       </c>
       <c r="AI172" t="s" s="2">
-        <v>498</v>
+        <v>63</v>
       </c>
       <c r="AJ172" t="s" s="2">
-        <v>499</v>
+        <v>535</v>
       </c>
       <c r="AK172" t="s" s="2">
         <v>151</v>
@@ -21806,7 +21792,7 @@
         <v>44</v>
       </c>
       <c r="AM172" t="s" s="2">
-        <v>44</v>
+        <v>536</v>
       </c>
       <c r="AN172" t="s" s="2">
         <v>44</v>
@@ -21814,7 +21800,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>500</v>
+        <v>537</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" t="s" s="2">
@@ -21837,13 +21823,13 @@
         <v>44</v>
       </c>
       <c r="J173" t="s" s="2">
-        <v>53</v>
+        <v>226</v>
       </c>
       <c r="K173" t="s" s="2">
-        <v>148</v>
+        <v>538</v>
       </c>
       <c r="L173" t="s" s="2">
-        <v>149</v>
+        <v>539</v>
       </c>
       <c r="M173" s="2"/>
       <c r="N173" s="2"/>
@@ -21894,7 +21880,7 @@
         <v>44</v>
       </c>
       <c r="AE173" t="s" s="2">
-        <v>150</v>
+        <v>537</v>
       </c>
       <c r="AF173" t="s" s="2">
         <v>42</v>
@@ -21906,13 +21892,13 @@
         <v>44</v>
       </c>
       <c r="AI173" t="s" s="2">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="AJ173" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="AK173" t="s" s="2">
         <v>151</v>
-      </c>
-      <c r="AK173" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="AL173" t="s" s="2">
         <v>44</v>
@@ -21926,11 +21912,11 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>501</v>
+        <v>541</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" t="s" s="2">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="D174" s="2"/>
       <c r="E174" t="s" s="2">
@@ -21949,18 +21935,20 @@
         <v>44</v>
       </c>
       <c r="J174" t="s" s="2">
-        <v>96</v>
+        <v>489</v>
       </c>
       <c r="K174" t="s" s="2">
-        <v>186</v>
+        <v>542</v>
       </c>
       <c r="L174" t="s" s="2">
-        <v>187</v>
+        <v>543</v>
       </c>
       <c r="M174" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N174" s="2"/>
+        <v>544</v>
+      </c>
+      <c r="N174" t="s" s="2">
+        <v>545</v>
+      </c>
       <c r="O174" t="s" s="2">
         <v>44</v>
       </c>
@@ -22008,7 +21996,7 @@
         <v>44</v>
       </c>
       <c r="AE174" t="s" s="2">
-        <v>154</v>
+        <v>541</v>
       </c>
       <c r="AF174" t="s" s="2">
         <v>42</v>
@@ -22020,13 +22008,13 @@
         <v>44</v>
       </c>
       <c r="AI174" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ174" t="s" s="2">
-        <v>151</v>
+        <v>546</v>
       </c>
       <c r="AK174" t="s" s="2">
-        <v>44</v>
+        <v>547</v>
       </c>
       <c r="AL174" t="s" s="2">
         <v>44</v>
@@ -22040,43 +22028,39 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>502</v>
+        <v>548</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
-        <v>503</v>
+        <v>44</v>
       </c>
       <c r="D175" s="2"/>
       <c r="E175" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F175" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G175" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H175" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I175" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J175" t="s" s="2">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="K175" t="s" s="2">
-        <v>504</v>
+        <v>148</v>
       </c>
       <c r="L175" t="s" s="2">
-        <v>505</v>
-      </c>
-      <c r="M175" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N175" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="M175" s="2"/>
+      <c r="N175" s="2"/>
       <c r="O175" t="s" s="2">
         <v>44</v>
       </c>
@@ -22124,22 +22108,22 @@
         <v>44</v>
       </c>
       <c r="AE175" t="s" s="2">
-        <v>506</v>
+        <v>150</v>
       </c>
       <c r="AF175" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG175" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH175" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI175" t="s" s="2">
-        <v>102</v>
+        <v>44</v>
       </c>
       <c r="AJ175" t="s" s="2">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="AK175" t="s" s="2">
         <v>44</v>
@@ -22156,11 +22140,11 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>507</v>
+        <v>549</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="D176" s="2"/>
       <c r="E176" t="s" s="2">
@@ -22179,18 +22163,18 @@
         <v>44</v>
       </c>
       <c r="J176" t="s" s="2">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="K176" t="s" s="2">
-        <v>508</v>
+        <v>186</v>
       </c>
       <c r="L176" t="s" s="2">
-        <v>509</v>
-      </c>
-      <c r="M176" s="2"/>
-      <c r="N176" t="s" s="2">
-        <v>510</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="M176" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="N176" s="2"/>
       <c r="O176" t="s" s="2">
         <v>44</v>
       </c>
@@ -22214,13 +22198,13 @@
         <v>44</v>
       </c>
       <c r="W176" t="s" s="2">
-        <v>346</v>
+        <v>44</v>
       </c>
       <c r="X176" t="s" s="2">
-        <v>511</v>
+        <v>44</v>
       </c>
       <c r="Y176" t="s" s="2">
-        <v>512</v>
+        <v>44</v>
       </c>
       <c r="Z176" t="s" s="2">
         <v>44</v>
@@ -22238,7 +22222,7 @@
         <v>44</v>
       </c>
       <c r="AE176" t="s" s="2">
-        <v>507</v>
+        <v>154</v>
       </c>
       <c r="AF176" t="s" s="2">
         <v>42</v>
@@ -22250,19 +22234,19 @@
         <v>44</v>
       </c>
       <c r="AI176" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ176" t="s" s="2">
-        <v>513</v>
+        <v>151</v>
       </c>
       <c r="AK176" t="s" s="2">
-        <v>151</v>
+        <v>44</v>
       </c>
       <c r="AL176" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM176" t="s" s="2">
-        <v>514</v>
+        <v>44</v>
       </c>
       <c r="AN176" t="s" s="2">
         <v>44</v>
@@ -22270,40 +22254,42 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>515</v>
+        <v>550</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
-        <v>44</v>
+        <v>499</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F177" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G177" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H177" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I177" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J177" t="s" s="2">
-        <v>382</v>
+        <v>96</v>
       </c>
       <c r="K177" t="s" s="2">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="M177" s="2"/>
+        <v>501</v>
+      </c>
+      <c r="M177" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N177" t="s" s="2">
-        <v>518</v>
+        <v>130</v>
       </c>
       <c r="O177" t="s" s="2">
         <v>44</v>
@@ -22352,31 +22338,31 @@
         <v>44</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG177" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH177" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI177" t="s" s="2">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="AJ177" t="s" s="2">
-        <v>387</v>
+        <v>94</v>
       </c>
       <c r="AK177" t="s" s="2">
-        <v>151</v>
+        <v>44</v>
       </c>
       <c r="AL177" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM177" t="s" s="2">
-        <v>519</v>
+        <v>44</v>
       </c>
       <c r="AN177" t="s" s="2">
         <v>44</v>
@@ -22384,7 +22370,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>520</v>
+        <v>551</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22392,10 +22378,10 @@
       </c>
       <c r="D178" s="2"/>
       <c r="E178" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F178" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G178" t="s" s="2">
         <v>44</v>
@@ -22407,19 +22393,19 @@
         <v>44</v>
       </c>
       <c r="J178" t="s" s="2">
-        <v>391</v>
+        <v>174</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>521</v>
+        <v>552</v>
       </c>
       <c r="L178" t="s" s="2">
-        <v>522</v>
+        <v>553</v>
       </c>
       <c r="M178" t="s" s="2">
-        <v>523</v>
+        <v>554</v>
       </c>
       <c r="N178" t="s" s="2">
-        <v>395</v>
+        <v>555</v>
       </c>
       <c r="O178" t="s" s="2">
         <v>44</v>
@@ -22444,13 +22430,11 @@
         <v>44</v>
       </c>
       <c r="W178" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X178" t="s" s="2">
-        <v>44</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="X178" s="2"/>
       <c r="Y178" t="s" s="2">
-        <v>44</v>
+        <v>556</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>44</v>
@@ -22468,13 +22452,13 @@
         <v>44</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>520</v>
+        <v>551</v>
       </c>
       <c r="AF178" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AG178" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH178" t="s" s="2">
         <v>44</v>
@@ -22483,16 +22467,16 @@
         <v>63</v>
       </c>
       <c r="AJ178" t="s" s="2">
-        <v>396</v>
+        <v>557</v>
       </c>
       <c r="AK178" t="s" s="2">
-        <v>151</v>
+        <v>558</v>
       </c>
       <c r="AL178" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM178" t="s" s="2">
-        <v>524</v>
+        <v>559</v>
       </c>
       <c r="AN178" t="s" s="2">
         <v>44</v>
@@ -22500,7 +22484,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>525</v>
+        <v>560</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22523,17 +22507,19 @@
         <v>44</v>
       </c>
       <c r="J179" t="s" s="2">
-        <v>459</v>
+        <v>369</v>
       </c>
       <c r="K179" t="s" s="2">
-        <v>526</v>
+        <v>561</v>
       </c>
       <c r="L179" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="M179" s="2"/>
+        <v>562</v>
+      </c>
+      <c r="M179" t="s" s="2">
+        <v>563</v>
+      </c>
       <c r="N179" t="s" s="2">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="O179" t="s" s="2">
         <v>44</v>
@@ -22582,7 +22568,7 @@
         <v>44</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>525</v>
+        <v>560</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>42</v>
@@ -22597,16 +22583,16 @@
         <v>63</v>
       </c>
       <c r="AJ179" t="s" s="2">
-        <v>464</v>
+        <v>565</v>
       </c>
       <c r="AK179" t="s" s="2">
-        <v>151</v>
+        <v>566</v>
       </c>
       <c r="AL179" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM179" t="s" s="2">
-        <v>529</v>
+        <v>567</v>
       </c>
       <c r="AN179" t="s" s="2">
         <v>44</v>
@@ -22614,18 +22600,18 @@
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>530</v>
+        <v>568</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
-        <v>44</v>
+        <v>569</v>
       </c>
       <c r="D180" s="2"/>
       <c r="E180" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F180" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G180" t="s" s="2">
         <v>44</v>
@@ -22637,18 +22623,18 @@
         <v>44</v>
       </c>
       <c r="J180" t="s" s="2">
-        <v>71</v>
+        <v>570</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>400</v>
+        <v>571</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>531</v>
-      </c>
-      <c r="M180" s="2"/>
-      <c r="N180" t="s" s="2">
-        <v>532</v>
-      </c>
+        <v>572</v>
+      </c>
+      <c r="M180" t="s" s="2">
+        <v>573</v>
+      </c>
+      <c r="N180" s="2"/>
       <c r="O180" t="s" s="2">
         <v>44</v>
       </c>
@@ -22672,13 +22658,13 @@
         <v>44</v>
       </c>
       <c r="W180" t="s" s="2">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="X180" t="s" s="2">
-        <v>404</v>
+        <v>44</v>
       </c>
       <c r="Y180" t="s" s="2">
-        <v>405</v>
+        <v>44</v>
       </c>
       <c r="Z180" t="s" s="2">
         <v>44</v>
@@ -22696,13 +22682,13 @@
         <v>44</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>530</v>
+        <v>568</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG180" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH180" t="s" s="2">
         <v>44</v>
@@ -22711,7 +22697,7 @@
         <v>63</v>
       </c>
       <c r="AJ180" t="s" s="2">
-        <v>406</v>
+        <v>574</v>
       </c>
       <c r="AK180" t="s" s="2">
         <v>151</v>
@@ -22720,7 +22706,7 @@
         <v>44</v>
       </c>
       <c r="AM180" t="s" s="2">
-        <v>533</v>
+        <v>575</v>
       </c>
       <c r="AN180" t="s" s="2">
         <v>44</v>
@@ -22728,7 +22714,7 @@
     </row>
     <row r="181" hidden="true">
       <c r="A181" t="s" s="2">
-        <v>534</v>
+        <v>576</v>
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
@@ -22748,20 +22734,22 @@
         <v>44</v>
       </c>
       <c r="I181" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J181" t="s" s="2">
         <v>233</v>
       </c>
       <c r="K181" t="s" s="2">
-        <v>535</v>
+        <v>577</v>
       </c>
       <c r="L181" t="s" s="2">
-        <v>536</v>
-      </c>
-      <c r="M181" s="2"/>
+        <v>578</v>
+      </c>
+      <c r="M181" t="s" s="2">
+        <v>579</v>
+      </c>
       <c r="N181" t="s" s="2">
-        <v>537</v>
+        <v>580</v>
       </c>
       <c r="O181" t="s" s="2">
         <v>44</v>
@@ -22810,7 +22798,7 @@
         <v>44</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>534</v>
+        <v>576</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>42</v>
@@ -22819,22 +22807,22 @@
         <v>51</v>
       </c>
       <c r="AH181" t="s" s="2">
-        <v>538</v>
+        <v>44</v>
       </c>
       <c r="AI181" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ181" t="s" s="2">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="AK181" t="s" s="2">
-        <v>151</v>
+        <v>581</v>
       </c>
       <c r="AL181" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM181" t="s" s="2">
-        <v>540</v>
+        <v>44</v>
       </c>
       <c r="AN181" t="s" s="2">
         <v>44</v>
@@ -22842,7 +22830,7 @@
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>541</v>
+        <v>582</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
@@ -22853,28 +22841,32 @@
         <v>42</v>
       </c>
       <c r="F182" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G182" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H182" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I182" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J182" t="s" s="2">
-        <v>226</v>
+        <v>489</v>
       </c>
       <c r="K182" t="s" s="2">
-        <v>542</v>
+        <v>583</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>543</v>
-      </c>
-      <c r="M182" s="2"/>
-      <c r="N182" s="2"/>
+        <v>584</v>
+      </c>
+      <c r="M182" t="s" s="2">
+        <v>585</v>
+      </c>
+      <c r="N182" t="s" s="2">
+        <v>586</v>
+      </c>
       <c r="O182" t="s" s="2">
         <v>44</v>
       </c>
@@ -22922,13 +22914,13 @@
         <v>44</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>541</v>
+        <v>582</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG182" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH182" t="s" s="2">
         <v>44</v>
@@ -22937,7 +22929,7 @@
         <v>63</v>
       </c>
       <c r="AJ182" t="s" s="2">
-        <v>544</v>
+        <v>587</v>
       </c>
       <c r="AK182" t="s" s="2">
         <v>151</v>
@@ -22954,7 +22946,7 @@
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>545</v>
+        <v>588</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
@@ -22965,7 +22957,7 @@
         <v>42</v>
       </c>
       <c r="F183" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G183" t="s" s="2">
         <v>44</v>
@@ -22977,20 +22969,16 @@
         <v>44</v>
       </c>
       <c r="J183" t="s" s="2">
-        <v>493</v>
+        <v>53</v>
       </c>
       <c r="K183" t="s" s="2">
-        <v>546</v>
+        <v>148</v>
       </c>
       <c r="L183" t="s" s="2">
-        <v>547</v>
-      </c>
-      <c r="M183" t="s" s="2">
-        <v>548</v>
-      </c>
-      <c r="N183" t="s" s="2">
-        <v>549</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="M183" s="2"/>
+      <c r="N183" s="2"/>
       <c r="O183" t="s" s="2">
         <v>44</v>
       </c>
@@ -23038,25 +23026,25 @@
         <v>44</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>545</v>
+        <v>150</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG183" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH183" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI183" t="s" s="2">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="AJ183" t="s" s="2">
-        <v>550</v>
+        <v>151</v>
       </c>
       <c r="AK183" t="s" s="2">
-        <v>551</v>
+        <v>44</v>
       </c>
       <c r="AL183" t="s" s="2">
         <v>44</v>
@@ -23070,18 +23058,18 @@
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>552</v>
+        <v>589</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="D184" s="2"/>
       <c r="E184" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F184" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G184" t="s" s="2">
         <v>44</v>
@@ -23093,15 +23081,17 @@
         <v>44</v>
       </c>
       <c r="J184" t="s" s="2">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="K184" t="s" s="2">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="L184" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="M184" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="M184" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="N184" s="2"/>
       <c r="O184" t="s" s="2">
         <v>44</v>
@@ -23150,19 +23140,19 @@
         <v>44</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG184" t="s" s="2">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AH184" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI184" t="s" s="2">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="AJ184" t="s" s="2">
         <v>151</v>
@@ -23182,11 +23172,11 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>553</v>
+        <v>590</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
-        <v>126</v>
+        <v>499</v>
       </c>
       <c r="D185" s="2"/>
       <c r="E185" t="s" s="2">
@@ -23199,24 +23189,26 @@
         <v>44</v>
       </c>
       <c r="H185" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="I185" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J185" t="s" s="2">
         <v>96</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>186</v>
+        <v>500</v>
       </c>
       <c r="L185" t="s" s="2">
-        <v>187</v>
+        <v>501</v>
       </c>
       <c r="M185" t="s" s="2">
         <v>129</v>
       </c>
-      <c r="N185" s="2"/>
+      <c r="N185" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="O185" t="s" s="2">
         <v>44</v>
       </c>
@@ -23264,7 +23256,7 @@
         <v>44</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>154</v>
+        <v>502</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>42</v>
@@ -23279,7 +23271,7 @@
         <v>102</v>
       </c>
       <c r="AJ185" t="s" s="2">
-        <v>151</v>
+        <v>94</v>
       </c>
       <c r="AK185" t="s" s="2">
         <v>44</v>
@@ -23296,43 +23288,41 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>554</v>
+        <v>591</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
-        <v>503</v>
+        <v>44</v>
       </c>
       <c r="D186" s="2"/>
       <c r="E186" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F186" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G186" t="s" s="2">
         <v>44</v>
       </c>
       <c r="H186" t="s" s="2">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I186" t="s" s="2">
         <v>52</v>
       </c>
       <c r="J186" t="s" s="2">
-        <v>96</v>
+        <v>592</v>
       </c>
       <c r="K186" t="s" s="2">
-        <v>504</v>
+        <v>593</v>
       </c>
       <c r="L186" t="s" s="2">
-        <v>505</v>
+        <v>594</v>
       </c>
       <c r="M186" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N186" t="s" s="2">
-        <v>130</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="N186" s="2"/>
       <c r="O186" t="s" s="2">
         <v>44</v>
       </c>
@@ -23380,31 +23370,31 @@
         <v>44</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>506</v>
+        <v>591</v>
       </c>
       <c r="AF186" t="s" s="2">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AG186" t="s" s="2">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AH186" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI186" t="s" s="2">
-        <v>102</v>
+        <v>63</v>
       </c>
       <c r="AJ186" t="s" s="2">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="AK186" t="s" s="2">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="AL186" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM186" t="s" s="2">
-        <v>44</v>
+        <v>596</v>
       </c>
       <c r="AN186" t="s" s="2">
         <v>44</v>
@@ -23412,7 +23402,7 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>555</v>
+        <v>597</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
@@ -23432,23 +23422,19 @@
         <v>44</v>
       </c>
       <c r="I187" t="s" s="2">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="J187" t="s" s="2">
-        <v>174</v>
+        <v>71</v>
       </c>
       <c r="K187" t="s" s="2">
-        <v>556</v>
+        <v>598</v>
       </c>
       <c r="L187" t="s" s="2">
-        <v>557</v>
-      </c>
-      <c r="M187" t="s" s="2">
-        <v>558</v>
-      </c>
-      <c r="N187" t="s" s="2">
-        <v>559</v>
-      </c>
+        <v>599</v>
+      </c>
+      <c r="M187" s="2"/>
+      <c r="N187" s="2"/>
       <c r="O187" t="s" s="2">
         <v>44</v>
       </c>
@@ -23472,11 +23458,13 @@
         <v>44</v>
       </c>
       <c r="W187" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="X187" s="2"/>
+        <v>168</v>
+      </c>
+      <c r="X187" t="s" s="2">
+        <v>599</v>
+      </c>
       <c r="Y187" t="s" s="2">
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="Z187" t="s" s="2">
         <v>44</v>
@@ -23494,7 +23482,7 @@
         <v>44</v>
       </c>
       <c r="AE187" t="s" s="2">
-        <v>555</v>
+        <v>597</v>
       </c>
       <c r="AF187" t="s" s="2">
         <v>51</v>
@@ -23509,1053 +23497,23 @@
         <v>63</v>
       </c>
       <c r="AJ187" t="s" s="2">
-        <v>561</v>
+        <v>601</v>
       </c>
       <c r="AK187" t="s" s="2">
-        <v>562</v>
+        <v>151</v>
       </c>
       <c r="AL187" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AM187" t="s" s="2">
-        <v>563</v>
+        <v>44</v>
       </c>
       <c r="AN187" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="188" hidden="true">
-      <c r="A188" t="s" s="2">
-        <v>564</v>
-      </c>
-      <c r="B188" s="2"/>
-      <c r="C188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D188" s="2"/>
-      <c r="E188" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F188" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="G188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J188" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="K188" t="s" s="2">
-        <v>565</v>
-      </c>
-      <c r="L188" t="s" s="2">
-        <v>566</v>
-      </c>
-      <c r="M188" t="s" s="2">
-        <v>567</v>
-      </c>
-      <c r="N188" t="s" s="2">
-        <v>568</v>
-      </c>
-      <c r="O188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P188" s="2"/>
-      <c r="Q188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE188" t="s" s="2">
-        <v>564</v>
-      </c>
-      <c r="AF188" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG188" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI188" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AJ188" t="s" s="2">
-        <v>569</v>
-      </c>
-      <c r="AK188" t="s" s="2">
-        <v>570</v>
-      </c>
-      <c r="AL188" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM188" t="s" s="2">
-        <v>571</v>
-      </c>
-      <c r="AN188" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="189" hidden="true">
-      <c r="A189" t="s" s="2">
-        <v>572</v>
-      </c>
-      <c r="B189" s="2"/>
-      <c r="C189" t="s" s="2">
-        <v>573</v>
-      </c>
-      <c r="D189" s="2"/>
-      <c r="E189" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F189" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J189" t="s" s="2">
-        <v>574</v>
-      </c>
-      <c r="K189" t="s" s="2">
-        <v>575</v>
-      </c>
-      <c r="L189" t="s" s="2">
-        <v>576</v>
-      </c>
-      <c r="M189" t="s" s="2">
-        <v>577</v>
-      </c>
-      <c r="N189" s="2"/>
-      <c r="O189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P189" s="2"/>
-      <c r="Q189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE189" t="s" s="2">
-        <v>572</v>
-      </c>
-      <c r="AF189" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG189" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI189" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AJ189" t="s" s="2">
-        <v>578</v>
-      </c>
-      <c r="AK189" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="AL189" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM189" t="s" s="2">
-        <v>579</v>
-      </c>
-      <c r="AN189" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="190" hidden="true">
-      <c r="A190" t="s" s="2">
-        <v>580</v>
-      </c>
-      <c r="B190" s="2"/>
-      <c r="C190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D190" s="2"/>
-      <c r="E190" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F190" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="G190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I190" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="J190" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="K190" t="s" s="2">
-        <v>581</v>
-      </c>
-      <c r="L190" t="s" s="2">
-        <v>582</v>
-      </c>
-      <c r="M190" t="s" s="2">
-        <v>583</v>
-      </c>
-      <c r="N190" t="s" s="2">
-        <v>584</v>
-      </c>
-      <c r="O190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P190" s="2"/>
-      <c r="Q190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE190" t="s" s="2">
-        <v>580</v>
-      </c>
-      <c r="AF190" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG190" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI190" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AJ190" t="s" s="2">
-        <v>539</v>
-      </c>
-      <c r="AK190" t="s" s="2">
-        <v>585</v>
-      </c>
-      <c r="AL190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM190" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN190" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="191" hidden="true">
-      <c r="A191" t="s" s="2">
-        <v>586</v>
-      </c>
-      <c r="B191" s="2"/>
-      <c r="C191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D191" s="2"/>
-      <c r="E191" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F191" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H191" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="I191" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="J191" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="K191" t="s" s="2">
-        <v>587</v>
-      </c>
-      <c r="L191" t="s" s="2">
-        <v>588</v>
-      </c>
-      <c r="M191" t="s" s="2">
-        <v>589</v>
-      </c>
-      <c r="N191" t="s" s="2">
-        <v>590</v>
-      </c>
-      <c r="O191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P191" s="2"/>
-      <c r="Q191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE191" t="s" s="2">
-        <v>586</v>
-      </c>
-      <c r="AF191" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG191" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI191" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AJ191" t="s" s="2">
-        <v>591</v>
-      </c>
-      <c r="AK191" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="AL191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM191" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN191" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="192" hidden="true">
-      <c r="A192" t="s" s="2">
-        <v>592</v>
-      </c>
-      <c r="B192" s="2"/>
-      <c r="C192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D192" s="2"/>
-      <c r="E192" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F192" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="G192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J192" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="K192" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="L192" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="M192" s="2"/>
-      <c r="N192" s="2"/>
-      <c r="O192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P192" s="2"/>
-      <c r="Q192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE192" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="AF192" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG192" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AJ192" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="AK192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM192" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN192" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="193" hidden="true">
-      <c r="A193" t="s" s="2">
-        <v>593</v>
-      </c>
-      <c r="B193" s="2"/>
-      <c r="C193" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="D193" s="2"/>
-      <c r="E193" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F193" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="J193" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="K193" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="L193" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="M193" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N193" s="2"/>
-      <c r="O193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P193" s="2"/>
-      <c r="Q193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE193" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AF193" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG193" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI193" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="AJ193" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="AK193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM193" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN193" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="194" hidden="true">
-      <c r="A194" t="s" s="2">
-        <v>594</v>
-      </c>
-      <c r="B194" s="2"/>
-      <c r="C194" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="D194" s="2"/>
-      <c r="E194" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="F194" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="G194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H194" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="I194" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="J194" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="K194" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="L194" t="s" s="2">
-        <v>505</v>
-      </c>
-      <c r="M194" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N194" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="O194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P194" s="2"/>
-      <c r="Q194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE194" t="s" s="2">
-        <v>506</v>
-      </c>
-      <c r="AF194" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG194" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AH194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI194" t="s" s="2">
-        <v>102</v>
-      </c>
-      <c r="AJ194" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AK194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM194" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN194" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="195" hidden="true">
-      <c r="A195" t="s" s="2">
-        <v>595</v>
-      </c>
-      <c r="B195" s="2"/>
-      <c r="C195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D195" s="2"/>
-      <c r="E195" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="F195" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="G195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I195" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="J195" t="s" s="2">
-        <v>596</v>
-      </c>
-      <c r="K195" t="s" s="2">
-        <v>597</v>
-      </c>
-      <c r="L195" t="s" s="2">
-        <v>598</v>
-      </c>
-      <c r="M195" t="s" s="2">
-        <v>599</v>
-      </c>
-      <c r="N195" s="2"/>
-      <c r="O195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P195" s="2"/>
-      <c r="Q195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="X195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Y195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="Z195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE195" t="s" s="2">
-        <v>595</v>
-      </c>
-      <c r="AF195" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG195" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI195" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AJ195" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="AK195" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="AL195" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM195" t="s" s="2">
-        <v>600</v>
-      </c>
-      <c r="AN195" t="s" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="196" hidden="true">
-      <c r="A196" t="s" s="2">
-        <v>601</v>
-      </c>
-      <c r="B196" s="2"/>
-      <c r="C196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D196" s="2"/>
-      <c r="E196" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="F196" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="G196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="H196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="I196" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="J196" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="K196" t="s" s="2">
-        <v>602</v>
-      </c>
-      <c r="L196" t="s" s="2">
-        <v>603</v>
-      </c>
-      <c r="M196" s="2"/>
-      <c r="N196" s="2"/>
-      <c r="O196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P196" s="2"/>
-      <c r="Q196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="R196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="S196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W196" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="X196" t="s" s="2">
-        <v>603</v>
-      </c>
-      <c r="Y196" t="s" s="2">
-        <v>604</v>
-      </c>
-      <c r="Z196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AA196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AB196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AC196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AD196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AE196" t="s" s="2">
-        <v>601</v>
-      </c>
-      <c r="AF196" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AG196" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="AH196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI196" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="AJ196" t="s" s="2">
-        <v>605</v>
-      </c>
-      <c r="AK196" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="AL196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM196" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN196" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN196">
+  <autoFilter ref="A1:AN187">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -24565,7 +23523,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI195">
+  <conditionalFormatting sqref="A2:AI186">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>